<commit_message>
ps3 游戏列表更新到 Burnout™ Paradise The Ultimate Box psv 游戏列表更新到 Virtua Tennis 4:World Tour Edition 游戏机收入更新到 2018-8-17 游戏目录网站rp 更新了橙色字体 增加gamedoc系统说明书
</commit_message>
<xml_diff>
--- a/游戏机收入.xlsx
+++ b/游戏机收入.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2278" uniqueCount="1388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2297" uniqueCount="1405">
   <si>
     <t>商品名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -5572,15 +5572,83 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>平顶山</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>面交</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>锦艺城面交3ds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>平顶山,要红色发黑色退了10元</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ps2原装光枪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>喜猪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>面交</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>转转</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>广东惠州</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>淘宝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>福建福州</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>md手柄2个+fc N制4手柄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>微信</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>买买提</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ps4 pro战神日版套装</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>咸鱼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>郑州二七面交</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>送给胖龙当维修费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ossc套件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>支付宝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>胖龙做的</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5702,7 +5770,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5916,7 +5984,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -6038,6 +6106,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
@@ -6406,10 +6480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R633"/>
+  <dimension ref="A1:R638"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A558" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H565" sqref="H565"/>
+    <sheetView tabSelected="1" topLeftCell="A610" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B636" sqref="B636"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -6644,25 +6718,39 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="6">
         <v>42287</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="7">
         <v>600</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="7">
         <v>20</v>
       </c>
-      <c r="K8">
+      <c r="G8" s="6">
+        <v>43304</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>1390</v>
+      </c>
+      <c r="I8" s="7">
+        <v>360</v>
+      </c>
+      <c r="J8" s="7">
+        <v>0</v>
+      </c>
+      <c r="K8" s="8">
         <f t="shared" si="0"/>
-        <v>-620</v>
-      </c>
+        <v>-260</v>
+      </c>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
     </row>
     <row r="9" spans="1:14">
       <c r="A9">
@@ -27325,21 +27413,40 @@
       <c r="A554">
         <v>554</v>
       </c>
-      <c r="B554" s="1">
+      <c r="B554" s="6">
         <v>43074</v>
       </c>
-      <c r="C554" s="5" t="s">
+      <c r="C554" s="7" t="s">
         <v>1143</v>
       </c>
-      <c r="D554" s="5" t="s">
+      <c r="D554" s="7" t="s">
         <v>1117</v>
       </c>
-      <c r="E554" s="5">
+      <c r="E554" s="7">
         <v>50</v>
       </c>
-      <c r="K554" s="9">
+      <c r="F554" s="7">
+        <v>0</v>
+      </c>
+      <c r="G554" s="6">
+        <v>43339</v>
+      </c>
+      <c r="H554" s="7" t="s">
+        <v>1391</v>
+      </c>
+      <c r="I554" s="7">
+        <v>180</v>
+      </c>
+      <c r="J554" s="7">
+        <v>10</v>
+      </c>
+      <c r="K554" s="8">
         <f t="shared" si="9"/>
-        <v>-50</v>
+        <v>120</v>
+      </c>
+      <c r="L554" s="7"/>
+      <c r="M554" s="7" t="s">
+        <v>1392</v>
       </c>
       <c r="N554" t="s">
         <v>1155</v>
@@ -27539,21 +27646,40 @@
       <c r="A560">
         <v>560</v>
       </c>
-      <c r="B560" s="1">
+      <c r="B560" s="6">
         <v>43075</v>
       </c>
-      <c r="C560" s="5" t="s">
+      <c r="C560" s="7" t="s">
         <v>1148</v>
       </c>
-      <c r="D560" s="5" t="s">
+      <c r="D560" s="7" t="s">
         <v>1117</v>
       </c>
-      <c r="E560" s="5">
+      <c r="E560" s="7">
         <v>40</v>
       </c>
-      <c r="K560" s="9">
+      <c r="F560" s="7">
+        <v>0</v>
+      </c>
+      <c r="G560" s="6">
+        <v>43308</v>
+      </c>
+      <c r="H560" s="7" t="s">
+        <v>1391</v>
+      </c>
+      <c r="I560" s="7">
+        <v>40</v>
+      </c>
+      <c r="J560" s="7">
+        <v>0</v>
+      </c>
+      <c r="K560" s="8">
         <f t="shared" si="9"/>
-        <v>-40</v>
+        <v>0</v>
+      </c>
+      <c r="L560" s="7"/>
+      <c r="M560" s="7" t="s">
+        <v>1392</v>
       </c>
     </row>
     <row r="561" spans="1:14">
@@ -27648,31 +27774,34 @@
       <c r="A564">
         <v>564</v>
       </c>
-      <c r="B564" s="4">
+      <c r="B564" s="24">
         <v>43075</v>
       </c>
-      <c r="C564" s="5" t="s">
+      <c r="C564" s="25" t="s">
         <v>1156</v>
       </c>
-      <c r="D564" s="5" t="s">
+      <c r="D564" s="25" t="s">
         <v>1154</v>
       </c>
-      <c r="E564" s="5">
+      <c r="E564" s="25">
         <v>50</v>
       </c>
-      <c r="F564" s="5">
+      <c r="F564" s="25">
         <v>32</v>
       </c>
-      <c r="G564" s="5"/>
-      <c r="H564" s="5"/>
-      <c r="I564" s="5"/>
-      <c r="J564" s="5"/>
-      <c r="K564" s="9">
+      <c r="G564" s="25"/>
+      <c r="H564" s="25"/>
+      <c r="I564" s="25"/>
+      <c r="J564" s="25"/>
+      <c r="K564" s="26">
         <f t="shared" si="9"/>
         <v>-82</v>
       </c>
-      <c r="L564" s="5"/>
-      <c r="M564" s="5"/>
+      <c r="L564" s="25"/>
+      <c r="M564" s="25"/>
+      <c r="N564" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="565" spans="1:14">
       <c r="A565">
@@ -27697,7 +27826,7 @@
         <v>43274</v>
       </c>
       <c r="H565" s="7" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="I565" s="7">
         <v>480</v>
@@ -27711,7 +27840,7 @@
       </c>
       <c r="L565" s="7"/>
       <c r="M565" s="7" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="566" spans="1:14">
@@ -29211,24 +29340,40 @@
       <c r="A606">
         <v>606</v>
       </c>
-      <c r="B606" s="1">
+      <c r="B606" s="6">
         <v>43163</v>
       </c>
-      <c r="C606" s="9" t="s">
+      <c r="C606" s="8" t="s">
         <v>1308</v>
       </c>
-      <c r="D606" s="5" t="s">
+      <c r="D606" s="7" t="s">
         <v>1306</v>
       </c>
-      <c r="E606" s="5">
+      <c r="E606" s="7">
         <v>390</v>
       </c>
-      <c r="F606" s="5">
-        <v>0</v>
-      </c>
-      <c r="K606" s="9">
+      <c r="F606" s="7">
+        <v>0</v>
+      </c>
+      <c r="G606" s="6">
+        <v>43338</v>
+      </c>
+      <c r="H606" s="7" t="s">
+        <v>1393</v>
+      </c>
+      <c r="I606" s="7">
+        <v>602</v>
+      </c>
+      <c r="J606" s="7">
+        <v>28</v>
+      </c>
+      <c r="K606" s="21">
         <f t="shared" si="14"/>
-        <v>-390</v>
+        <v>184</v>
+      </c>
+      <c r="L606" s="7"/>
+      <c r="M606" s="7" t="s">
+        <v>1394</v>
       </c>
     </row>
     <row r="607" spans="1:13">
@@ -29884,7 +30029,7 @@
         <v>16</v>
       </c>
       <c r="K623" s="8">
-        <f t="shared" ref="K623:K631" si="23">I623-F623-E623-J623</f>
+        <f t="shared" ref="K623:K635" si="23">I623-F623-E623-J623</f>
         <v>24</v>
       </c>
       <c r="L623" s="7"/>
@@ -30111,7 +30256,7 @@
         <v>0</v>
       </c>
       <c r="F631" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G631" s="6">
         <v>43299</v>
@@ -30123,24 +30268,140 @@
       <c r="J631" s="7">
         <v>20</v>
       </c>
-      <c r="K631" s="41">
+      <c r="K631" s="8">
         <f t="shared" si="23"/>
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="L631" s="7"/>
       <c r="M631" s="7"/>
       <c r="N631" t="s">
-        <v>1385</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="632" spans="1:14">
       <c r="A632">
         <v>632</v>
       </c>
+      <c r="B632" s="1">
+        <v>43303</v>
+      </c>
+      <c r="C632" t="s">
+        <v>1388</v>
+      </c>
+      <c r="D632" t="s">
+        <v>1389</v>
+      </c>
+      <c r="E632">
+        <v>60</v>
+      </c>
+      <c r="F632">
+        <v>10</v>
+      </c>
+      <c r="K632" s="9">
+        <f t="shared" si="23"/>
+        <v>-70</v>
+      </c>
     </row>
     <row r="633" spans="1:14">
       <c r="A633">
         <v>633</v>
+      </c>
+      <c r="B633" s="41">
+        <v>43324</v>
+      </c>
+      <c r="C633" s="42" t="s">
+        <v>1395</v>
+      </c>
+      <c r="D633" s="42" t="s">
+        <v>1396</v>
+      </c>
+      <c r="E633" s="42">
+        <v>168</v>
+      </c>
+      <c r="F633" s="42">
+        <v>0</v>
+      </c>
+      <c r="G633" s="42"/>
+      <c r="H633" s="42"/>
+      <c r="I633" s="42"/>
+      <c r="J633" s="42"/>
+      <c r="K633" s="43">
+        <f t="shared" si="23"/>
+        <v>-168</v>
+      </c>
+      <c r="L633" s="42"/>
+      <c r="M633" s="42"/>
+      <c r="N633" t="s">
+        <v>1397</v>
+      </c>
+    </row>
+    <row r="634" spans="1:14">
+      <c r="A634">
+        <v>634</v>
+      </c>
+      <c r="B634" s="1">
+        <v>43329</v>
+      </c>
+      <c r="C634" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D634" t="s">
+        <v>1399</v>
+      </c>
+      <c r="E634">
+        <v>3500</v>
+      </c>
+      <c r="F634">
+        <v>10</v>
+      </c>
+      <c r="K634" s="9">
+        <f t="shared" si="23"/>
+        <v>-3510</v>
+      </c>
+      <c r="N634" t="s">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="635" spans="1:14">
+      <c r="A635">
+        <v>635</v>
+      </c>
+      <c r="B635" s="1">
+        <v>43266</v>
+      </c>
+      <c r="C635" t="s">
+        <v>1402</v>
+      </c>
+      <c r="D635" t="s">
+        <v>1403</v>
+      </c>
+      <c r="E635">
+        <v>500</v>
+      </c>
+      <c r="F635">
+        <v>0</v>
+      </c>
+      <c r="K635" s="9">
+        <f t="shared" si="23"/>
+        <v>-500</v>
+      </c>
+      <c r="N635" t="s">
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="636" spans="1:14">
+      <c r="A636">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="637" spans="1:14">
+      <c r="A637">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="638" spans="1:14">
+      <c r="A638">
+        <v>638</v>
       </c>
     </row>
   </sheetData>

</xml_diff>